<commit_message>
add chart and data to excel file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>tran dong nam</t>
   </si>
@@ -40,7 +40,7 @@
     <t>tran quang viet</t>
   </si>
   <si>
-    <t>19021392@vnu.edu.vn</t>
+    <t>19021337@vnu.edu.vn</t>
   </si>
   <si>
     <t>female</t>
@@ -52,7 +52,37 @@
     <t>nguyen thanh vinh</t>
   </si>
   <si>
-    <t>19021395@vnu.edu.vn</t>
+    <t>19021338@vnu.edu.vn</t>
+  </si>
+  <si>
+    <t>tran van a</t>
+  </si>
+  <si>
+    <t>19021339@vnu.edu.vn</t>
+  </si>
+  <si>
+    <t>tran van b</t>
+  </si>
+  <si>
+    <t>19021340@vnu.edu.vn</t>
+  </si>
+  <si>
+    <t>tran van c</t>
+  </si>
+  <si>
+    <t>19021341@vnu.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tran van d </t>
+  </si>
+  <si>
+    <t>19021342@vnu.edu.vn</t>
+  </si>
+  <si>
+    <t>tran van e</t>
+  </si>
+  <si>
+    <t>19021343@vnu.edu.vn</t>
   </si>
 </sst>
 </file>
@@ -88,17 +118,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -324,8 +357,8 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
-        <v>12345.0</v>
+      <c r="C1" s="2">
+        <v>1.2345678E7</v>
       </c>
       <c r="D1" s="1">
         <v>1.9021336E7</v>
@@ -336,7 +369,7 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="3">
         <v>36922.0</v>
       </c>
       <c r="H1" s="1">
@@ -351,8 +384,8 @@
       <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="3">
-        <v>3.0</v>
+      <c r="L1" s="2">
+        <v>2.8</v>
       </c>
       <c r="M1" s="1">
         <v>100.0</v>
@@ -368,43 +401,43 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
-        <v>12345.0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.9021392E7</v>
-      </c>
-      <c r="E2" s="1">
-        <v>35202.0</v>
+      <c r="C2" s="2">
+        <v>1.2345678E7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.9021337E7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>35201.0</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>36923.0</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>9.87654321E8</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="M2" s="1">
+      <c r="L2" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="M2" s="2">
         <v>100.0</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -412,49 +445,284 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1">
-        <v>12345.0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.9021395E7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>35203.0</v>
+      <c r="C3" s="2">
+        <v>1.2345678E7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.9021338E7</v>
+      </c>
+      <c r="E3" s="2">
+        <v>35201.0</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>36924.0</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>9.87654321E8</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="M3" s="2">
+        <v>100.0</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.2345678E7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.9021339E7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>35201.0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>36925.0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>9.87654321E8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="M4" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.2345678E7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.902134E7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>35201.0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>36926.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>9.87654321E8</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="2">
         <v>3.0</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M5" s="1">
         <v>100.0</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.2345678E7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.9021341E7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>35201.0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4">
+        <v>36927.0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>9.87654321E8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="M6" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.2345678E7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.9021342E7</v>
+      </c>
+      <c r="E7" s="1">
+        <v>35201.0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4">
+        <v>36928.0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>9.87654321E8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.2345678E7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.9021343E7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>35201.0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4">
+        <v>36929.0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>9.87654321E8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="M8" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>